<commit_message>
adding geo code buffer for faster geocoding, add data that will be used in evaluation model experiment into data/ csv file and raw data is in data/rawDataSet
</commit_message>
<xml_diff>
--- a/data/月度旅游距离与流量.xlsx
+++ b/data/月度旅游距离与流量.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -20,18 +20,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>旅游人次</t>
+    <t>Average Travel Distance</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>平均旅游距离</t>
+    <t>Travel Man-Time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -126,7 +126,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>平均旅游距离</c:v>
+                  <c:v>Average Travel Distance</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -201,6 +201,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0CEF-4B0A-8FED-0C1CDD51EB23}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -227,7 +232,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>旅游人次</c:v>
+                  <c:v>Travel Man-Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -310,6 +315,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0CEF-4B0A-8FED-0C1CDD51EB23}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -351,13 +361,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="zh-CN" altLang="en-US"/>
-                  <a:t>月份</a:t>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Month</a:t>
                 </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -471,13 +481,17 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="zh-CN" altLang="en-US"/>
-                  <a:t>平均旅游距离</a:t>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Average Travel</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t> Distance</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -570,13 +584,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="zh-CN" altLang="en-US"/>
-                  <a:t>旅游人次</a:t>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Travel Man-Time</a:t>
                 </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -672,9 +686,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.79834692715317612"/>
+          <c:x val="0.70059182867578373"/>
           <c:y val="2.7777777777777776E-2"/>
-          <c:w val="0.18717343621349522"/>
+          <c:w val="0.28492839950637383"/>
           <c:h val="0.12384368620589092"/>
         </c:manualLayout>
       </c:layout>
@@ -1323,7 +1337,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1398,6 +1412,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1433,6 +1464,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1612,20 +1660,23 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>